<commit_message>
[DEV] Closing Quality Chapter
</commit_message>
<xml_diff>
--- a/Imagens_Diagramas_Tabelas.xlsx
+++ b/Imagens_Diagramas_Tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -540,6 +540,990 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="34" name="Grupo 33"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2057400" y="666751"/>
+          <a:ext cx="8048625" cy="4333875"/>
+          <a:chOff x="2057400" y="666751"/>
+          <a:chExt cx="8048625" cy="4333875"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Retângulo de cantos arredondados 1"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5000626" y="2352675"/>
+            <a:ext cx="2190750" cy="990601"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1600">
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>ISO/IEC 25010:2011</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="pt-BR" sz="900">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100">
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Qualdade</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1100" baseline="0">
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> do Produto</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1100">
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Retângulo de cantos arredondados 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6705600" y="695326"/>
+            <a:ext cx="2181225" cy="628650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+              <a:alpha val="45000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>FUNCIONALIDADE</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Retângulo de cantos arredondados 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7924800" y="1714501"/>
+            <a:ext cx="2181225" cy="628650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+              <a:alpha val="45000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>CONFIABILIDADE</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Retângulo de cantos arredondados 4"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7924800" y="3343276"/>
+            <a:ext cx="2181225" cy="628650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+              <a:alpha val="45000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>OPERABILIDADE</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Retângulo de cantos arredondados 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6705600" y="4371976"/>
+            <a:ext cx="2181225" cy="628650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+              <a:alpha val="45000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>SEGURANÇA</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Retângulo de cantos arredondados 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3286125" y="666751"/>
+            <a:ext cx="2181225" cy="628650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+              <a:alpha val="45000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>PORTABILIDADE</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Retângulo de cantos arredondados 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3286125" y="4343401"/>
+            <a:ext cx="2181225" cy="628650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+              <a:alpha val="45000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>COMPATIBILIDADE</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Retângulo de cantos arredondados 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2057400" y="1714501"/>
+            <a:ext cx="2181225" cy="628650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+              <a:alpha val="45000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>CAPACIDADE DE MANUTENÇÃO</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Retângulo de cantos arredondados 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2057400" y="3343276"/>
+            <a:ext cx="2181225" cy="628650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+              <a:alpha val="45000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="55000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>EFICIÊNCIA</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="12" name="Conector reto 11"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="3"/>
+            <a:endCxn id="3" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="7191376" y="1323976"/>
+            <a:ext cx="604837" cy="1524000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="14" name="Conector reto 13"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="3"/>
+            <a:endCxn id="4" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="7191376" y="2028826"/>
+            <a:ext cx="733424" cy="819150"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="17" name="Conector reto 16"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="3"/>
+            <a:endCxn id="5" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7191376" y="2847976"/>
+            <a:ext cx="733424" cy="809625"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="18" name="Conector reto 17"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="3"/>
+            <a:endCxn id="6" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7191376" y="2847976"/>
+            <a:ext cx="604837" cy="1524000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="21" name="Conector reto 20"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="1"/>
+            <a:endCxn id="8" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="4376738" y="2847976"/>
+            <a:ext cx="623888" cy="1495425"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="24" name="Conector reto 23"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="1"/>
+            <a:endCxn id="10" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="3148013" y="2847976"/>
+            <a:ext cx="1852613" cy="495300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="27" name="Conector reto 26"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="1"/>
+            <a:endCxn id="9" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="4238625" y="2028826"/>
+            <a:ext cx="762001" cy="819150"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="30" name="Conector reto 29"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="1"/>
+            <a:endCxn id="7" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="4376738" y="1295401"/>
+            <a:ext cx="623888" cy="1552575"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="31750">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -833,7 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -848,11 +1832,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[DEV] Setup CMMI Chapter
</commit_message>
<xml_diff>
--- a/Imagens_Diagramas_Tabelas.xlsx
+++ b/Imagens_Diagramas_Tabelas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="1"/>
@@ -16,8 +16,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +54,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -637,7 +642,7 @@
                 <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>Qualdade</a:t>
+              <a:t>Qualidade</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" sz="1100" baseline="0">
@@ -1531,9 +1536,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1571,7 +1576,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1605,6 +1610,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1639,9 +1645,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1814,14 +1821,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1829,14 +1836,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1844,12 +1851,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
[DEV] Initial steps CMMI
</commit_message>
<xml_diff>
--- a/Imagens_Diagramas_Tabelas.xlsx
+++ b/Imagens_Diagramas_Tabelas.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -15,15 +15,174 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+  <si>
+    <t>Nível</t>
+  </si>
+  <si>
+    <t>Sigla</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>- Gestão da configuração</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>- Medição e Análise</t>
+  </si>
+  <si>
+    <t>PMC</t>
+  </si>
+  <si>
+    <t>- Projeto de Monitoramento e Controle</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>- Planejamento de Projetos</t>
+  </si>
+  <si>
+    <t>PPQA</t>
+  </si>
+  <si>
+    <t>- Processo e Produto Quality Assurance</t>
+  </si>
+  <si>
+    <t>REQM</t>
+  </si>
+  <si>
+    <t>- Gerenciamento de Requisitos</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>- Gerenciamento de acordo com o fornecedor</t>
+  </si>
+  <si>
+    <t>DAR</t>
+  </si>
+  <si>
+    <t>- Análise de decisão e resolução</t>
+  </si>
+  <si>
+    <t>IPM</t>
+  </si>
+  <si>
+    <t>- Gestão Integrada de Projetos</t>
+  </si>
+  <si>
+    <t>OPD</t>
+  </si>
+  <si>
+    <t>- Definição do Processo Organizacional</t>
+  </si>
+  <si>
+    <t>OPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Foco no Processo Organizacional </t>
+  </si>
+  <si>
+    <t>OT</t>
+  </si>
+  <si>
+    <t>- Treinamento Organizacional</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>- Integração de Produto</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>- Desenvolvimento de Requisitos</t>
+  </si>
+  <si>
+    <t>RSKM</t>
+  </si>
+  <si>
+    <t>- Gestão de Riscos</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>- Solução Técnica</t>
+  </si>
+  <si>
+    <t>VAL</t>
+  </si>
+  <si>
+    <t>- Validação</t>
+  </si>
+  <si>
+    <t>VER</t>
+  </si>
+  <si>
+    <t>- Verificação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPP </t>
+  </si>
+  <si>
+    <t>- Performance do Processo Organizacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QPM </t>
+  </si>
+  <si>
+    <t>- Projeto quantativamente gerenciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAR </t>
+  </si>
+  <si>
+    <t>- Análise e Resolução de Causas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPM </t>
+  </si>
+  <si>
+    <t>- Gestão de Desempenho Organizacional</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +205,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1536,9 +1726,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1576,7 +1766,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1610,7 +1800,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1645,10 +1834,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1821,14 +2009,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1836,14 +2024,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1851,13 +2039,259 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75">
+      <c r="A22" s="11">
+        <v>4</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75">
+      <c r="A23" s="11"/>
+      <c r="B23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75">
+      <c r="A25" s="11">
+        <v>5</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75">
+      <c r="A26" s="11"/>
+      <c r="B26" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A10:A20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A26"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[DEV] Initial Steps CMMI Chapter
</commit_message>
<xml_diff>
--- a/Imagens_Diagramas_Tabelas.xlsx
+++ b/Imagens_Diagramas_Tabelas.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -15,15 +15,174 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+  <si>
+    <t>Nível</t>
+  </si>
+  <si>
+    <t>Sigla</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>- Gestão da configuração</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>- Medição e Análise</t>
+  </si>
+  <si>
+    <t>PMC</t>
+  </si>
+  <si>
+    <t>- Projeto de Monitoramento e Controle</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>- Planejamento de Projetos</t>
+  </si>
+  <si>
+    <t>PPQA</t>
+  </si>
+  <si>
+    <t>- Processo e Produto Quality Assurance</t>
+  </si>
+  <si>
+    <t>REQM</t>
+  </si>
+  <si>
+    <t>- Gerenciamento de Requisitos</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>- Gerenciamento de acordo com o fornecedor</t>
+  </si>
+  <si>
+    <t>DAR</t>
+  </si>
+  <si>
+    <t>- Análise de decisão e resolução</t>
+  </si>
+  <si>
+    <t>IPM</t>
+  </si>
+  <si>
+    <t>- Gestão Integrada de Projetos</t>
+  </si>
+  <si>
+    <t>OPD</t>
+  </si>
+  <si>
+    <t>- Definição do Processo Organizacional</t>
+  </si>
+  <si>
+    <t>OPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Foco no Processo Organizacional </t>
+  </si>
+  <si>
+    <t>OT</t>
+  </si>
+  <si>
+    <t>- Treinamento Organizacional</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>- Integração de Produto</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>- Desenvolvimento de Requisitos</t>
+  </si>
+  <si>
+    <t>RSKM</t>
+  </si>
+  <si>
+    <t>- Gestão de Riscos</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>- Solução Técnica</t>
+  </si>
+  <si>
+    <t>VAL</t>
+  </si>
+  <si>
+    <t>- Validação</t>
+  </si>
+  <si>
+    <t>VER</t>
+  </si>
+  <si>
+    <t>- Verificação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPP </t>
+  </si>
+  <si>
+    <t>- Performance do Processo Organizacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QPM </t>
+  </si>
+  <si>
+    <t>- Projeto quantativamente gerenciado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAR </t>
+  </si>
+  <si>
+    <t>- Análise e Resolução de Causas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPM </t>
+  </si>
+  <si>
+    <t>- Gestão de Desempenho Organizacional</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +205,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1536,9 +1726,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1576,7 +1766,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1610,7 +1800,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1645,10 +1834,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1821,14 +2009,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1836,14 +2024,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1851,13 +2039,259 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75">
+      <c r="A22" s="11">
+        <v>4</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75">
+      <c r="A23" s="11"/>
+      <c r="B23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75">
+      <c r="A25" s="11">
+        <v>5</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75">
+      <c r="A26" s="11"/>
+      <c r="B26" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A10:A20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A26"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[DEV] Development CMMI Chapter
</commit_message>
<xml_diff>
--- a/Imagens_Diagramas_Tabelas.xlsx
+++ b/Imagens_Diagramas_Tabelas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19155" windowHeight="8505" activeTab="3"/>
@@ -163,8 +163,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1739,715 +1739,1209 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="15" name="Group 14"/>
+        <xdr:cNvPr id="41" name="Grupo 40"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1247775" y="66675"/>
-          <a:ext cx="4038600" cy="3533775"/>
-          <a:chOff x="1247775" y="66675"/>
-          <a:chExt cx="4038600" cy="3533775"/>
+          <a:off x="1247775" y="38100"/>
+          <a:ext cx="6362699" cy="3562350"/>
+          <a:chOff x="1247775" y="38100"/>
+          <a:chExt cx="6362699" cy="3562350"/>
         </a:xfrm>
       </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="15" name="Group 14"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1247775" y="66675"/>
+            <a:ext cx="4038600" cy="3533775"/>
+            <a:chOff x="1247775" y="66675"/>
+            <a:chExt cx="4038600" cy="3533775"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="Rectangle 1"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1247775" y="3086100"/>
+              <a:ext cx="1638300" cy="514350"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
+                <a:srgbClr val="000000">
+                  <a:alpha val="32000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="balanced" dir="t">
+                <a:rot lat="0" lon="0" rev="8700000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="190500" h="38100"/>
+            </a:sp3d>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Nível 1</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1200" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>INICIAL</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="Rectangle 2"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2438400" y="1666875"/>
+              <a:ext cx="1638300" cy="514350"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F5F793"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
+                <a:srgbClr val="000000">
+                  <a:alpha val="32000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="balanced" dir="t">
+                <a:rot lat="0" lon="0" rev="8700000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="190500" h="38100"/>
+            </a:sp3d>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Nível 3</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1200" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Definido</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="Rectangle 3"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1847850" y="2333625"/>
+              <a:ext cx="1638300" cy="514350"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
+                <a:srgbClr val="000000">
+                  <a:alpha val="32000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="balanced" dir="t">
+                <a:rot lat="0" lon="0" rev="8700000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="190500" h="38100"/>
+            </a:sp3d>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Nível 2</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1200" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Gerenciado</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="Rectangle 4"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3076575" y="809624"/>
+              <a:ext cx="1638300" cy="676275"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="DFF298"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
+                <a:srgbClr val="000000">
+                  <a:alpha val="32000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="balanced" dir="t">
+                <a:rot lat="0" lon="0" rev="8700000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="190500" h="38100"/>
+            </a:sp3d>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Nível 4</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1200" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Quantitativamente gerenciado</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Rectangle 5"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3648075" y="66675"/>
+              <a:ext cx="1638300" cy="514350"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
+                <a:srgbClr val="000000">
+                  <a:alpha val="32000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="balanced" dir="t">
+                <a:rot lat="0" lon="0" rev="8700000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="190500" h="38100"/>
+            </a:sp3d>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1000" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Nível 5 </a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1200" b="1">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>Otimizado</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="Bent Arrow 9"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1409700" y="2505075"/>
+              <a:ext cx="409575" cy="561975"/>
+            </a:xfrm>
+            <a:prstGeom prst="bentArrow">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="50000" endA="300" endPos="38500" dist="50800" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="Bent Arrow 11"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2000250" y="1828801"/>
+              <a:ext cx="409575" cy="485774"/>
+            </a:xfrm>
+            <a:prstGeom prst="bentArrow">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="50000" endA="300" endPos="38500" dist="50800" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="Bent Arrow 12"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2667000" y="1133476"/>
+              <a:ext cx="409575" cy="485774"/>
+            </a:xfrm>
+            <a:prstGeom prst="bentArrow">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="50000" endA="300" endPos="38500" dist="50800" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="Bent Arrow 13"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3248025" y="314326"/>
+              <a:ext cx="409575" cy="485774"/>
+            </a:xfrm>
+            <a:prstGeom prst="bentArrow">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:reflection blurRad="6350" stA="50000" endA="300" endPos="38500" dist="50800" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
+            </a:effectLst>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="dk1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" indent="0" algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="2" name="Rectangle 1"/>
-          <xdr:cNvSpPr/>
+          <xdr:cNvPr id="16" name="CaixaDeTexto 15"/>
+          <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="1247775" y="3086100"/>
-            <a:ext cx="1638300" cy="514350"/>
+            <a:off x="3171825" y="3076575"/>
+            <a:ext cx="2647950" cy="504825"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
           <a:solidFill>
-            <a:schemeClr val="accent2">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
+            <a:schemeClr val="lt1"/>
           </a:solidFill>
-          <a:ln>
+          <a:ln w="9525" cmpd="sng">
             <a:noFill/>
           </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
-              <a:srgbClr val="000000">
-                <a:alpha val="32000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="balanced" dir="t">
-              <a:rot lat="0" lon="0" rev="8700000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="190500" h="38100"/>
-          </a:sp3d>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:fillRef>
           <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="dk1"/>
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:pPr marL="0" indent="0" algn="l"/>
             <a:r>
-              <a:rPr lang="en-GB" sz="1000" b="1">
+              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="dk1"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>Nível 1</a:t>
+              <a:t>Ad Hoc, Ocasionalmente caótico</a:t>
             </a:r>
           </a:p>
           <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:pPr marL="0" indent="0" algn="l"/>
             <a:r>
-              <a:rPr lang="en-GB" sz="1200" b="1">
+              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:schemeClr val="dk1"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>INICIAL</a:t>
+              <a:t>Poucos processos definidos</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="18" name="Conector reto 17"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="2" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2886075" y="3343275"/>
+            <a:ext cx="609600" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 2"/>
-          <xdr:cNvSpPr/>
+          <xdr:cNvPr id="21" name="CaixaDeTexto 20"/>
+          <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="2438400" y="1666875"/>
-            <a:ext cx="1638300" cy="514350"/>
+            <a:off x="3495675" y="2257424"/>
+            <a:ext cx="2552700" cy="619125"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
           <a:solidFill>
-            <a:srgbClr val="F5F793"/>
+            <a:schemeClr val="lt1"/>
           </a:solidFill>
-          <a:ln>
+          <a:ln w="9525" cmpd="sng">
             <a:noFill/>
           </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
-              <a:srgbClr val="000000">
-                <a:alpha val="32000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="balanced" dir="t">
-              <a:rot lat="0" lon="0" rev="8700000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="190500" h="38100"/>
-          </a:sp3d>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:fillRef>
           <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="dk1"/>
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="ctr"/>
+            <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="en-GB" sz="1000" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
+                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>Nível 3</a:t>
+              <a:t>Gerenciamento básico dos projetos.</a:t>
             </a:r>
           </a:p>
           <a:p>
-            <a:pPr algn="ctr"/>
+            <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="en-GB" sz="1200" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:rPr lang="pt-BR" sz="1000" b="1" u="none" baseline="0">
+                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>Definido</a:t>
+              <a:t>(Custo, Cronograma, Prazo)</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="34" name="Conector reto 33"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3486150" y="2562225"/>
+            <a:ext cx="609600" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Rectangle 3"/>
-          <xdr:cNvSpPr/>
+          <xdr:cNvPr id="35" name="CaixaDeTexto 34"/>
+          <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="1847850" y="2333625"/>
-            <a:ext cx="1638300" cy="514350"/>
+            <a:off x="4229100" y="1543049"/>
+            <a:ext cx="2476500" cy="752476"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
           <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
+            <a:schemeClr val="lt1"/>
           </a:solidFill>
-          <a:ln>
+          <a:ln w="9525" cmpd="sng">
             <a:noFill/>
           </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
-              <a:srgbClr val="000000">
-                <a:alpha val="32000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="balanced" dir="t">
-              <a:rot lat="0" lon="0" rev="8700000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="190500" h="38100"/>
-          </a:sp3d>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:fillRef>
           <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="dk1"/>
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="en-GB" sz="1000" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
+                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>Nível 2</a:t>
+              <a:t>Processo de software para gestão e desenvolvimento é documentado, padronizado e integrado em um processo global para a organização</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1200" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Gerenciado</a:t>
-            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1000" b="1" u="none" baseline="0">
+              <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="36" name="Conector reto 35"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4067175" y="1914525"/>
+            <a:ext cx="609600" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Rectangle 4"/>
-          <xdr:cNvSpPr/>
+          <xdr:cNvPr id="37" name="CaixaDeTexto 36"/>
+          <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="3076575" y="809624"/>
-            <a:ext cx="1638300" cy="676275"/>
+            <a:off x="4952999" y="838199"/>
+            <a:ext cx="2162175" cy="752476"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
           <a:solidFill>
-            <a:srgbClr val="DFF298"/>
+            <a:schemeClr val="lt1"/>
           </a:solidFill>
-          <a:ln>
+          <a:ln w="9525" cmpd="sng">
             <a:noFill/>
           </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
-              <a:srgbClr val="000000">
-                <a:alpha val="32000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="balanced" dir="t">
-              <a:rot lat="0" lon="0" rev="8700000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="190500" h="38100"/>
-          </a:sp3d>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:fillRef>
           <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="dk1"/>
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
+            <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="en-GB" sz="1000" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
+                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
               </a:rPr>
-              <a:t>Nível 4</a:t>
+              <a:t>Processos e produtos são quantitativamente compreendidos e controlados</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1200" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Quantitativamente gerenciado</a:t>
-            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1000" b="1" u="none" baseline="0">
+              <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="38" name="Conector reto 37"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4705350" y="1143000"/>
+            <a:ext cx="609600" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Rectangle 5"/>
-          <xdr:cNvSpPr/>
+          <xdr:cNvPr id="39" name="CaixaDeTexto 38"/>
+          <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="3648075" y="66675"/>
-            <a:ext cx="1638300" cy="514350"/>
+            <a:off x="5448299" y="38100"/>
+            <a:ext cx="2162175" cy="752476"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
           <a:solidFill>
-            <a:srgbClr val="92D050"/>
+            <a:schemeClr val="lt1"/>
           </a:solidFill>
-          <a:ln>
+          <a:ln w="9525" cmpd="sng">
             <a:noFill/>
           </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
-              <a:srgbClr val="000000">
-                <a:alpha val="32000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="balanced" dir="t">
-              <a:rot lat="0" lon="0" rev="8700000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="190500" h="38100"/>
-          </a:sp3d>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:fillRef>
           <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
+            <a:scrgbClr r="0" g="0" b="0"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="dk1"/>
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1000" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Nível 5 </a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1200" b="1">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Otimizado</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="Bent Arrow 9"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1409700" y="2505075"/>
-            <a:ext cx="409575" cy="561975"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentArrow">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="50000"/>
-              <a:lumOff val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst>
-            <a:reflection blurRad="6350" stA="50000" endA="300" endPos="38500" dist="50800" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
-          </a:effectLst>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="dk1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1000" b="1" u="none">
+                <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Melhoria contínua dos processos através de feedback quantitativo</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1000" b="1" u="none" baseline="0">
+              <a:latin typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Tahoma" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Tahoma" pitchFamily="34" charset="0"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="Bent Arrow 11"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="40" name="Conector reto 39"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="2000250" y="1828801"/>
-            <a:ext cx="409575" cy="485774"/>
+            <a:off x="5276850" y="333375"/>
+            <a:ext cx="609600" cy="1"/>
           </a:xfrm>
-          <a:prstGeom prst="bentArrow">
+          <a:prstGeom prst="line">
             <a:avLst/>
           </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="50000"/>
-              <a:lumOff val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
+          <a:ln w="25400">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:solidFill>
           </a:ln>
-          <a:effectLst>
-            <a:reflection blurRad="6350" stA="50000" endA="300" endPos="38500" dist="50800" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
-          </a:effectLst>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="dk1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
           </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="dk1"/>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
           </a:fillRef>
           <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
+            <a:schemeClr val="accent1"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="tx1"/>
           </a:fontRef>
         </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="l"/>
-            <a:endParaRPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="Bent Arrow 12"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2667000" y="1133476"/>
-            <a:ext cx="409575" cy="485774"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentArrow">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="50000"/>
-              <a:lumOff val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst>
-            <a:reflection blurRad="6350" stA="50000" endA="300" endPos="38500" dist="50800" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
-          </a:effectLst>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="dk1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="l"/>
-            <a:endParaRPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="Bent Arrow 13"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3248025" y="314326"/>
-            <a:ext cx="409575" cy="485774"/>
-          </a:xfrm>
-          <a:prstGeom prst="bentArrow">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="50000"/>
-              <a:lumOff val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst>
-            <a:reflection blurRad="6350" stA="50000" endA="300" endPos="38500" dist="50800" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
-          </a:effectLst>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="dk1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" indent="0" algn="l"/>
-            <a:endParaRPr lang="en-GB" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
+      </xdr:cxnSp>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -2455,9 +2949,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2495,7 +2989,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2529,7 +3023,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2564,10 +3057,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2740,14 +3232,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -2755,14 +3247,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="D4" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -2770,21 +3262,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2795,7 +3287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="10">
         <v>2</v>
       </c>
@@ -2806,7 +3298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -2815,7 +3307,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="10"/>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -2824,7 +3316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="10"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -2833,7 +3325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="10"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -2842,7 +3334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="10"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
@@ -2851,7 +3343,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="10"/>
       <c r="B8" s="4" t="s">
         <v>15</v>
@@ -2860,12 +3352,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="10">
         <v>3</v>
       </c>
@@ -2876,7 +3368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="10"/>
       <c r="B11" s="4" t="s">
         <v>19</v>
@@ -2885,7 +3377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="10"/>
       <c r="B12" s="4" t="s">
         <v>21</v>
@@ -2894,7 +3386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="10"/>
       <c r="B13" s="4" t="s">
         <v>23</v>
@@ -2903,7 +3395,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="10"/>
       <c r="B14" s="4" t="s">
         <v>25</v>
@@ -2912,7 +3404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="10"/>
       <c r="B15" s="4" t="s">
         <v>27</v>
@@ -2921,7 +3413,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="10"/>
       <c r="B16" s="4" t="s">
         <v>29</v>
@@ -2930,7 +3422,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="10"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
@@ -2939,7 +3431,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="10"/>
       <c r="B18" s="4" t="s">
         <v>33</v>
@@ -2948,7 +3440,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="10"/>
       <c r="B19" s="4" t="s">
         <v>35</v>
@@ -2957,7 +3449,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="10"/>
       <c r="B20" s="4" t="s">
         <v>37</v>
@@ -2966,12 +3458,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.75">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15.75">
       <c r="A22" s="11">
         <v>4</v>
       </c>
@@ -2982,7 +3474,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.75">
       <c r="A23" s="11"/>
       <c r="B23" s="7" t="s">
         <v>41</v>
@@ -2991,12 +3483,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.75">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15.75">
       <c r="A25" s="11">
         <v>5</v>
       </c>
@@ -3007,7 +3499,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15.75">
       <c r="A26" s="11"/>
       <c r="B26" s="7" t="s">
         <v>45</v>
@@ -3028,14 +3520,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>